<commit_message>
data visuals and regressions
</commit_message>
<xml_diff>
--- a/data/Age_1564.xlsx
+++ b/data/Age_1564.xlsx
@@ -14,9 +14,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">European Union</t>
-  </si>
-  <si>
     <t xml:space="preserve">Austria</t>
   </si>
   <si>
@@ -53,21 +50,24 @@
     <t xml:space="preserve">Greece</t>
   </si>
   <si>
+    <t xml:space="preserve">Hungary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ireland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Italy</t>
   </si>
   <si>
-    <t xml:space="preserve">Ireland</t>
+    <t xml:space="preserve">Latvia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lithuania</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg</t>
   </si>
   <si>
-    <t xml:space="preserve">Lithuania</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Latvia</t>
-  </si>
-  <si>
     <t xml:space="preserve">Malta</t>
   </si>
   <si>
@@ -80,12 +80,15 @@
     <t xml:space="preserve">Portugal</t>
   </si>
   <si>
+    <t xml:space="preserve">Romania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovak Republic</t>
+  </si>
+  <si>
     <t xml:space="preserve">Slovenia</t>
   </si>
   <si>
-    <t xml:space="preserve">Slovak Republic</t>
-  </si>
-  <si>
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
@@ -93,9 +96,6 @@
   </si>
   <si>
     <t xml:space="preserve">United Kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hungary</t>
   </si>
   <si>
     <t xml:space="preserve">Created from: World Development Indicators
@@ -105,66 +105,69 @@
     <t xml:space="preserve">1996</t>
   </si>
   <si>
+    <t xml:space="preserve">67.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">67.3</t>
   </si>
   <si>
-    <t xml:space="preserve">67.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65.9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66.8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66.3</t>
+    <t xml:space="preserve">67.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.9</t>
   </si>
   <si>
     <t xml:space="preserve">69.7</t>
   </si>
   <si>
-    <t xml:space="preserve">66.9</t>
-  </si>
-  <si>
     <t xml:space="preserve">68.4</t>
   </si>
   <si>
@@ -192,12 +195,12 @@
     <t xml:space="preserve">68.1</t>
   </si>
   <si>
+    <t xml:space="preserve">67.9</t>
+  </si>
+  <si>
     <t xml:space="preserve">67.0</t>
   </si>
   <si>
-    <t xml:space="preserve">67.5</t>
-  </si>
-  <si>
     <t xml:space="preserve">69.8</t>
   </si>
   <si>
@@ -207,9 +210,6 @@
     <t xml:space="preserve">64.7</t>
   </si>
   <si>
-    <t xml:space="preserve">67.9</t>
-  </si>
-  <si>
     <t xml:space="preserve">1998</t>
   </si>
   <si>
@@ -261,12 +261,12 @@
     <t xml:space="preserve">2000</t>
   </si>
   <si>
+    <t xml:space="preserve">69.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">70.1</t>
   </si>
   <si>
-    <t xml:space="preserve">69.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">64.3</t>
   </si>
   <si>
@@ -345,10 +345,10 @@
     <t xml:space="preserve">69.5</t>
   </si>
   <si>
+    <t xml:space="preserve">71.8</t>
+  </si>
+  <si>
     <t xml:space="preserve">70.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71.8</t>
   </si>
   <si>
     <t xml:space="preserve">2007</t>
@@ -673,7 +673,7 @@
         <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>66</v>
@@ -754,77 +754,77 @@
         <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="P2" s="4"/>
       <c r="Q2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="W2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="X2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>70</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="U2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="V2" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="W2" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="X2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y2" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="14.25" customHeight="1">
@@ -835,77 +835,77 @@
         <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="N3" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="P3" s="4"/>
       <c r="Q3" s="4" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="T3" s="4" t="s">
-        <v>31</v>
+        <v>108</v>
       </c>
       <c r="U3" s="4" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>47</v>
+        <v>123</v>
       </c>
       <c r="Y3" s="4" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="Z3" s="4" t="s">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="AA3" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="14.25" customHeight="1">
@@ -913,80 +913,80 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="J4" s="4" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="T4" s="4" t="s">
+      <c r="U4" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W4" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="U4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="X4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y4" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="Y4" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="Z4" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA4" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="14.25" customHeight="1">
@@ -994,80 +994,80 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="N5" s="4" t="s">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>102</v>
+        <v>31</v>
       </c>
       <c r="P5" s="4"/>
       <c r="Q5" s="4" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="T5" s="4" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="U5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="V5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="V5" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="W5" s="4" t="s">
-        <v>108</v>
+        <v>32</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>123</v>
+        <v>76</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="AA5" s="4" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="14.25" customHeight="1">
@@ -1078,77 +1078,77 @@
         <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>60</v>
+        <v>93</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>32</v>
+        <v>110</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="P6" s="4"/>
       <c r="Q6" s="4" t="s">
-        <v>60</v>
+        <v>119</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>39</v>
+        <v>119</v>
       </c>
       <c r="T6" s="4" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="U6" s="4" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="V6" s="4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="Y6" s="4" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="Z6" s="4" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="AA6" s="4" t="s">
-        <v>137</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="14.25" customHeight="1">
@@ -1159,77 +1159,77 @@
         <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>57</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>36</v>
+        <v>97</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
       <c r="P7" s="4"/>
       <c r="Q7" s="4" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>119</v>
+        <v>51</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="T7" s="4" t="s">
-        <v>98</v>
+        <v>41</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>111</v>
+        <v>56</v>
       </c>
       <c r="V7" s="4" t="s">
-        <v>94</v>
+        <v>50</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="Y7" s="4" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="Z7" s="4" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="AA7" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:27" ht="14.25" customHeight="1">
@@ -1240,77 +1240,77 @@
         <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>105</v>
+        <v>37</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>103</v>
+        <v>43</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>100</v>
+        <v>34</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="P8" s="4"/>
       <c r="Q8" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="T8" s="4" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="U8" s="4" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="V8" s="4" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="W8" s="4" t="s">
-        <v>48</v>
+        <v>125</v>
       </c>
       <c r="X8" s="4" t="s">
-        <v>43</v>
+        <v>139</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="Z8" s="4" t="s">
-        <v>127</v>
+        <v>53</v>
       </c>
       <c r="AA8" s="4" t="s">
-        <v>80</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1">
@@ -1321,77 +1321,77 @@
         <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="L9" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="N9" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="M9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="O9" s="4" t="s">
-        <v>91</v>
+        <v>56</v>
       </c>
       <c r="P9" s="4"/>
       <c r="Q9" s="4" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="T9" s="4" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="V9" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="W9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="X9" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y9" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="X9" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="Y9" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="Z9" s="4" t="s">
-        <v>52</v>
+        <v>130</v>
       </c>
       <c r="AA9" s="4" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1">
@@ -1402,77 +1402,77 @@
         <v>38</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>65</v>
+        <v>38</v>
       </c>
       <c r="N10" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="P10" s="4"/>
       <c r="Q10" s="4" t="s">
-        <v>31</v>
+        <v>101</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="T10" s="4" t="s">
-        <v>33</v>
+        <v>127</v>
       </c>
       <c r="U10" s="4" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="V10" s="4" t="s">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="Z10" s="4" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="AA10" s="4" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1">
@@ -1483,71 +1483,71 @@
         <v>39</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="P11" s="4"/>
       <c r="Q11" s="4" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="R11" s="4" t="s">
-        <v>46</v>
+        <v>123</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>40</v>
+        <v>125</v>
       </c>
       <c r="T11" s="4" t="s">
-        <v>127</v>
+        <v>53</v>
       </c>
       <c r="U11" s="4" t="s">
-        <v>72</v>
+        <v>129</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="W11" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="X11" s="4" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Z11" s="4" t="s">
         <v>146</v>
@@ -1564,77 +1564,77 @@
         <v>40</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="M12" s="4" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="P12" s="4"/>
       <c r="Q12" s="4" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="R12" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="V12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="X12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z12" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA12" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="S12" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="T12" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="U12" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="V12" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="W12" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="X12" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="Z12" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="AA12" s="4" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1">
@@ -1645,77 +1645,77 @@
         <v>41</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="I13" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="M13" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="N13" s="4" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="P13" s="4"/>
       <c r="Q13" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="R13" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>35</v>
+        <v>108</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="U13" s="4" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="V13" s="4" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="W13" s="4" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
       <c r="X13" s="4" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="Y13" s="4" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="Z13" s="4" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
       <c r="AA13" s="4" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1">
@@ -1723,80 +1723,80 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>44</v>
+        <v>88</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="P14" s="4"/>
       <c r="Q14" s="4" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="R14" s="4" t="s">
-        <v>43</v>
+        <v>88</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="U14" s="4" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="V14" s="4" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="W14" s="4" t="s">
-        <v>127</v>
+        <v>56</v>
       </c>
       <c r="X14" s="4" t="s">
-        <v>123</v>
+        <v>62</v>
       </c>
       <c r="Y14" s="4" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="Z14" s="4" t="s">
-        <v>137</v>
+        <v>44</v>
       </c>
       <c r="AA14" s="4" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1">
@@ -1807,77 +1807,77 @@
         <v>42</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="N15" s="4" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
       <c r="O15" s="4" t="s">
         <v>35</v>
       </c>
       <c r="P15" s="4"/>
       <c r="Q15" s="4" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="R15" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="V15" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="S15" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="T15" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="U15" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="V15" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="W15" s="4" t="s">
-        <v>137</v>
+        <v>59</v>
       </c>
       <c r="X15" s="4" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
       <c r="Y15" s="4" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="Z15" s="4" t="s">
-        <v>139</v>
+        <v>54</v>
       </c>
       <c r="AA15" s="4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1">
@@ -1885,80 +1885,80 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>36</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>84</v>
+        <v>43</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="O16" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="P16" s="4"/>
       <c r="Q16" s="4" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="R16" s="4" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="S16" s="4" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="U16" s="4" t="s">
-        <v>45</v>
+        <v>127</v>
       </c>
       <c r="V16" s="4" t="s">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="W16" s="4" t="s">
-        <v>58</v>
+        <v>137</v>
       </c>
       <c r="X16" s="4" t="s">
-        <v>81</v>
+        <v>125</v>
       </c>
       <c r="Y16" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z16" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA16" s="4" t="s">
         <v>64</v>
-      </c>
-      <c r="Z16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="AA16" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:27" ht="14.25" customHeight="1">
@@ -1966,80 +1966,80 @@
         <v>16</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="N17" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="O17" s="4" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="P17" s="4"/>
       <c r="Q17" s="4" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="S17" s="4" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="U17" s="4" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="V17" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="W17" s="4" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="X17" s="4" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="Y17" s="4" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="Z17" s="4" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="AA17" s="4" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:27" ht="14.25" customHeight="1">
@@ -2047,62 +2047,62 @@
         <v>17</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L18" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="M18" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="N18" s="4" t="s">
         <v>77</v>
       </c>
       <c r="O18" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="P18" s="4"/>
       <c r="Q18" s="4" t="s">
         <v>69</v>
       </c>
       <c r="R18" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="T18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="U18" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="U18" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="V18" s="4" t="s">
         <v>68</v>
@@ -2111,13 +2111,13 @@
         <v>70</v>
       </c>
       <c r="X18" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y18" s="4" t="s">
         <v>95</v>
       </c>
       <c r="Z18" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AA18" s="4" t="s">
         <v>72</v>
@@ -2128,80 +2128,80 @@
         <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="I19" s="4" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="P19" s="4"/>
       <c r="Q19" s="4" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="R19" s="4" t="s">
-        <v>31</v>
+        <v>79</v>
       </c>
       <c r="S19" s="4" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="T19" s="4" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="U19" s="4" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="V19" s="4" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="W19" s="4" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="X19" s="4" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="Y19" s="4" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="Z19" s="4" t="s">
-        <v>132</v>
+        <v>78</v>
       </c>
       <c r="AA19" s="4" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:27" ht="14.25" customHeight="1">
@@ -2209,28 +2209,28 @@
         <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>77</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J20" s="4" t="s">
         <v>102</v>
@@ -2255,25 +2255,25 @@
         <v>106</v>
       </c>
       <c r="R20" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S20" s="4" t="s">
         <v>79</v>
       </c>
       <c r="T20" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="U20" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="V20" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="W20" s="4" t="s">
         <v>70</v>
       </c>
       <c r="X20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Y20" s="4" t="s">
         <v>95</v>
@@ -2290,13 +2290,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>69</v>
@@ -2305,59 +2305,59 @@
         <v>69</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>77</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="S21" s="4" t="s">
         <v>70</v>
       </c>
       <c r="T21" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U21" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V21" s="4" t="s">
         <v>108</v>
       </c>
       <c r="W21" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="X21" s="4" t="s">
         <v>81</v>
       </c>
       <c r="Y21" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="Z21" s="4" t="s">
         <v>127</v>
@@ -2371,19 +2371,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E22" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>88</v>
@@ -2423,7 +2423,7 @@
         <v>97</v>
       </c>
       <c r="T22" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="U22" s="4" t="s">
         <v>78</v>
@@ -2435,16 +2435,16 @@
         <v>88</v>
       </c>
       <c r="X22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y22" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Z22" s="4" t="s">
         <v>68</v>
       </c>
       <c r="AA22" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:27" ht="14.25" customHeight="1">
@@ -2452,13 +2452,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>77</v>
@@ -2470,19 +2470,19 @@
         <v>77</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>50</v>
@@ -2491,7 +2491,7 @@
         <v>68</v>
       </c>
       <c r="O23" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P23" s="4"/>
       <c r="Q23" s="4" t="s">
@@ -2501,16 +2501,16 @@
         <v>101</v>
       </c>
       <c r="S23" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="T23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U23" s="4" t="s">
         <v>95</v>
       </c>
       <c r="V23" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W23" s="4" t="s">
         <v>76</v>
@@ -2519,7 +2519,7 @@
         <v>73</v>
       </c>
       <c r="Y23" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Z23" s="4" t="s">
         <v>123</v>
@@ -2536,77 +2536,77 @@
         <v>49</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="F24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>92</v>
-      </c>
       <c r="L24" s="4" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="O24" s="4" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="P24" s="4"/>
       <c r="Q24" s="4" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="R24" s="4" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="S24" s="4" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="T24" s="4" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="U24" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V24" s="4" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="W24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="X24" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="X24" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="Y24" s="4" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="Z24" s="4" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="AA24" s="4" t="s">
-        <v>80</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:27" ht="14.25" customHeight="1">
@@ -2617,22 +2617,22 @@
         <v>50</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>89</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I25" s="4" t="s">
         <v>98</v>
@@ -2644,7 +2644,7 @@
         <v>107</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M25" s="4" t="s">
         <v>115</v>
@@ -2663,7 +2663,7 @@
         <v>115</v>
       </c>
       <c r="S25" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T25" s="4" t="s">
         <v>107</v>
@@ -2684,7 +2684,7 @@
         <v>88</v>
       </c>
       <c r="Z25" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AA25" s="4" t="s">
         <v>77</v>
@@ -2698,77 +2698,77 @@
         <v>51</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>67</v>
+        <v>92</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="O26" s="4" t="s">
-        <v>42</v>
+        <v>89</v>
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
       <c r="R26" s="4" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="S26" s="4" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="T26" s="4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="U26" s="4" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="V26" s="4" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="W26" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="X26" s="4" t="s">
-        <v>101</v>
+        <v>37</v>
       </c>
       <c r="Y26" s="4" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="Z26" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="AA26" s="4" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:27" ht="14.25" customHeight="1">
@@ -2779,77 +2779,77 @@
         <v>52</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>72</v>
+        <v>35</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="K27" s="4" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>95</v>
+        <v>35</v>
       </c>
       <c r="O27" s="4" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="4" t="s">
-        <v>108</v>
+        <v>40</v>
       </c>
       <c r="R27" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="S27" s="4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="T27" s="4" t="s">
-        <v>125</v>
+        <v>31</v>
       </c>
       <c r="U27" s="4" t="s">
-        <v>130</v>
+        <v>46</v>
       </c>
       <c r="V27" s="4" t="s">
-        <v>129</v>
+        <v>70</v>
       </c>
       <c r="W27" s="4" t="s">
-        <v>133</v>
+        <v>47</v>
       </c>
       <c r="X27" s="4" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="Y27" s="4" t="s">
-        <v>144</v>
+        <v>32</v>
       </c>
       <c r="Z27" s="4" t="s">
-        <v>140</v>
+        <v>43</v>
       </c>
       <c r="AA27" s="4" t="s">
-        <v>143</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:27" ht="14.25" customHeight="1">
@@ -2863,74 +2863,74 @@
         <v>64</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H28" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="4" t="s">
+      <c r="I28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="L28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="N28" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="O28" s="4" t="s">
-        <v>38</v>
+        <v>95</v>
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="4" t="s">
-        <v>45</v>
+        <v>108</v>
       </c>
       <c r="R28" s="4" t="s">
-        <v>43</v>
+        <v>76</v>
       </c>
       <c r="S28" s="4" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>76</v>
+        <v>125</v>
       </c>
       <c r="U28" s="4" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
       <c r="V28" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="W28" s="4" t="s">
-        <v>85</v>
+        <v>133</v>
       </c>
       <c r="X28" s="4" t="s">
-        <v>80</v>
+        <v>136</v>
       </c>
       <c r="Y28" s="4" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="Z28" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AA28" s="4" t="s">
-        <v>63</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:27" ht="14.25" customHeight="1">
@@ -2938,80 +2938,80 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>65</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>59</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="O29" s="4" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="P29" s="4"/>
       <c r="Q29" s="4" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="R29" s="4" t="s">
-        <v>88</v>
+        <v>42</v>
       </c>
       <c r="S29" s="4" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="T29" s="4" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="U29" s="4" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="V29" s="4" t="s">
-        <v>59</v>
+        <v>127</v>
       </c>
       <c r="W29" s="4" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="X29" s="4" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="Y29" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="Z29" s="4" t="s">
-        <v>45</v>
+        <v>139</v>
       </c>
       <c r="AA29" s="4" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:27" ht="27.75" customHeight="1">

</xml_diff>